<commit_message>
fix tai chinh va cong thuc 50%
</commit_message>
<xml_diff>
--- a/kpi nam/DU THAO KPI 2021 khoa ngoai than kinh.xlsx
+++ b/kpi nam/DU THAO KPI 2021 khoa ngoai than kinh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/kpi/kpi nam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9BFABC-86A4-0841-81F1-F5FE08CAE910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1D1832-D7C3-2E4D-92A5-D64E6CDD4A80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="22360" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,18 +236,6 @@
   </si>
   <si>
     <t>KPI=KQ/90%*100%</t>
-  </si>
-  <si>
-    <t>90% bệnh nhân xuất viện trước 4 giờ</t>
-  </si>
-  <si>
-    <t>KPI=100%*I(KQ&gt;90%)</t>
-  </si>
-  <si>
-    <t>Tỷ lệ BN xuất viện trước 4 giờ</t>
-  </si>
-  <si>
-    <t>90%</t>
   </si>
   <si>
     <t>KPI=KQ/60%*100%*I(KQ&gt;=50%)</t>
@@ -350,10 +338,44 @@
     <t>DỰ THẢO KPI NGOẠI THẦN KINH - NĂM 2021</t>
   </si>
   <si>
-    <t>KPI=KQ/2*100%*(1/2*I(BV không đạt))</t>
-  </si>
-  <si>
     <t>Ngày ...../...../2021</t>
+  </si>
+  <si>
+    <t>KPI=KQ/2*100%*(1/2*I(BV không đạt) + I(BV đạt))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tổng </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">định phí </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">không vượt quá 105% so với 2020 </t>
+    </r>
+  </si>
+  <si>
+    <t>Tổng chi thường xuyên</t>
+  </si>
+  <si>
+    <t>KPI=1%/KQ*100%*I(KQ&lt;=105%)</t>
+  </si>
+  <si>
+    <t>105%</t>
   </si>
 </sst>
 </file>
@@ -910,6 +932,12 @@
     <xf numFmtId="9" fontId="25" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -921,12 +949,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1215,10 +1237,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1877,7 +1899,7 @@
     <row r="2" spans="1:14" s="6" customFormat="1" ht="33" x14ac:dyDescent="0.2">
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
@@ -2061,29 +2083,29 @@
       <c r="A8" s="52">
         <v>4</v>
       </c>
-      <c r="B8" s="99" t="s">
-        <v>69</v>
+      <c r="B8" s="53" t="s">
+        <v>97</v>
       </c>
       <c r="C8" s="54">
         <v>0.2</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="F8" s="93" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="58" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H8" s="57" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="67" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="J8" s="68"/>
       <c r="K8" s="64"/>
@@ -2105,7 +2127,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F9" s="93" t="s">
         <v>67</v>
@@ -2150,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C11" s="54">
         <v>0.2</v>
@@ -2159,7 +2181,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F11" s="93" t="s">
         <v>67</v>
@@ -2183,17 +2205,17 @@
       <c r="A12" s="52">
         <v>2</v>
       </c>
-      <c r="B12" s="99" t="s">
-        <v>87</v>
+      <c r="B12" s="95" t="s">
+        <v>83</v>
       </c>
       <c r="C12" s="54">
         <v>0.2</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F12" s="93" t="s">
         <v>67</v>
@@ -2224,10 +2246,10 @@
         <v>0.2</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F13" s="93" t="s">
         <v>67</v>
@@ -2261,7 +2283,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F14" s="93" t="s">
         <v>67</v>
@@ -2295,7 +2317,7 @@
         <v>32</v>
       </c>
       <c r="E15" s="94" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F15" s="93" t="s">
         <v>67</v>
@@ -2383,7 +2405,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="56" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F18" s="93" t="s">
         <v>67</v>
@@ -2407,17 +2429,17 @@
       <c r="A19" s="52">
         <v>3</v>
       </c>
-      <c r="B19" s="99" t="s">
-        <v>86</v>
+      <c r="B19" s="95" t="s">
+        <v>82</v>
       </c>
       <c r="C19" s="54">
         <v>0.2</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19" s="93" t="s">
         <v>67</v>
@@ -2451,7 +2473,7 @@
         <v>40</v>
       </c>
       <c r="E20" s="56" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" s="93" t="s">
         <v>67</v>
@@ -2476,16 +2498,16 @@
         <v>5</v>
       </c>
       <c r="B21" s="53" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C21" s="54">
         <v>0.2</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E21" s="56" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F21" s="93" t="s">
         <v>67</v>
@@ -2497,7 +2519,7 @@
         <v>41</v>
       </c>
       <c r="I21" s="67" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J21" s="62"/>
       <c r="K21" s="78"/>
@@ -2539,7 +2561,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="56" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F23" s="93" t="s">
         <v>67</v>
@@ -2564,16 +2586,16 @@
         <v>2</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C24" s="54">
         <v>0.2</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E24" s="56" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F24" s="93" t="s">
         <v>67</v>
@@ -2641,7 +2663,7 @@
         <v>51</v>
       </c>
       <c r="E26" s="56" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F26" s="93" t="s">
         <v>67</v>
@@ -2665,17 +2687,17 @@
       <c r="A27" s="52">
         <v>5</v>
       </c>
-      <c r="B27" s="100" t="s">
-        <v>92</v>
+      <c r="B27" s="96" t="s">
+        <v>88</v>
       </c>
       <c r="C27" s="54">
         <v>0.2</v>
       </c>
       <c r="D27" s="55" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E27" s="56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F27" s="93" t="s">
         <v>67</v>
@@ -2718,10 +2740,10 @@
     </row>
     <row r="29" spans="1:14" s="23" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="95"/>
+      <c r="C29" s="97"/>
       <c r="D29" s="24"/>
       <c r="E29" s="25"/>
       <c r="F29" s="25" t="s">
@@ -2729,28 +2751,28 @@
       </c>
       <c r="H29" s="25"/>
       <c r="I29" s="25"/>
-      <c r="J29" s="96" t="s">
+      <c r="J29" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="96"/>
-      <c r="L29" s="96"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
       <c r="M29" s="38"/>
       <c r="N29" s="26"/>
     </row>
     <row r="30" spans="1:14" s="23" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
-      <c r="B30" s="97"/>
-      <c r="C30" s="97"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="99"/>
       <c r="D30" s="20"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="98" t="s">
+      <c r="J30" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="98"/>
-      <c r="L30" s="98"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="100"/>
       <c r="M30" s="39"/>
       <c r="N30" s="26"/>
     </row>
@@ -2831,10 +2853,10 @@
     </row>
     <row r="36" spans="1:14" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="20"/>
-      <c r="B36" s="97" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="97"/>
+      <c r="B36" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="99"/>
       <c r="D36" s="20"/>
       <c r="E36" s="21"/>
       <c r="F36" s="21" t="s">
@@ -2842,11 +2864,11 @@
       </c>
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
-      <c r="J36" s="98" t="s">
+      <c r="J36" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="K36" s="98"/>
-      <c r="L36" s="98"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="100"/>
       <c r="M36" s="39"/>
       <c r="N36" s="29"/>
     </row>

</xml_diff>